<commit_message>
Increase compatibility with Tanzania pilot baseline data
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict_tanzania_pilot_baseline.xlsx
+++ b/inst/extdata/main_dict_tanzania_pilot_baseline.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="677">
   <si>
     <t>old</t>
   </si>
@@ -2046,6 +2046,15 @@
   </si>
   <si>
     <t>child_hfid_yn</t>
+  </si>
+  <si>
+    <t>crfs-t02a-a4_a_2</t>
+  </si>
+  <si>
+    <t>ms_name</t>
+  </si>
+  <si>
+    <t>a4_a_2</t>
   </si>
 </sst>
 </file>
@@ -2481,10 +2490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I232"/>
+  <dimension ref="A1:I233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4422,10 +4431,10 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="s">
-        <v>374</v>
+        <v>674</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>41</v>
+        <v>675</v>
       </c>
       <c r="C74" s="2">
         <v>0</v>
@@ -4443,15 +4452,18 @@
         <v>0</v>
       </c>
       <c r="H74" s="9" t="s">
-        <v>214</v>
+        <v>676</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>645</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C75" s="2">
         <v>0</v>
@@ -4469,122 +4481,122 @@
         <v>0</v>
       </c>
       <c r="H75" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C76" s="2">
+        <v>0</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1</v>
+      </c>
+      <c r="E76" s="4">
+        <v>0</v>
+      </c>
+      <c r="F76" s="4">
+        <v>0</v>
+      </c>
+      <c r="G76" s="3">
+        <v>0</v>
+      </c>
+      <c r="H76" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B77" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C76" s="2">
-        <v>0</v>
-      </c>
-      <c r="D76" s="2">
-        <v>1</v>
-      </c>
-      <c r="E76" s="4">
-        <v>0</v>
-      </c>
-      <c r="F76" s="4">
-        <v>0</v>
-      </c>
-      <c r="G76" s="3">
-        <v>0</v>
-      </c>
-      <c r="H76" s="9" t="s">
+      <c r="C77" s="2">
+        <v>0</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
+      <c r="E77" s="4">
+        <v>0</v>
+      </c>
+      <c r="F77" s="4">
+        <v>0</v>
+      </c>
+      <c r="G77" s="3">
+        <v>0</v>
+      </c>
+      <c r="H77" s="9" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="19" t="s">
-        <v>512</v>
-      </c>
-      <c r="B77" s="19" t="s">
-        <v>513</v>
-      </c>
-      <c r="C77" s="2">
-        <v>1</v>
-      </c>
-      <c r="D77" s="2">
-        <v>1</v>
-      </c>
-      <c r="E77" s="4">
-        <v>1</v>
-      </c>
-      <c r="F77" s="4">
-        <v>1</v>
-      </c>
-      <c r="G77" s="3">
-        <v>1</v>
-      </c>
-      <c r="H77" s="11" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="B78" s="19" t="s">
+        <v>513</v>
+      </c>
+      <c r="C78" s="2">
+        <v>1</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
+      <c r="E78" s="4">
+        <v>1</v>
+      </c>
+      <c r="F78" s="4">
+        <v>1</v>
+      </c>
+      <c r="G78" s="3">
+        <v>1</v>
+      </c>
+      <c r="H78" s="11" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="19" t="s">
         <v>514</v>
       </c>
-      <c r="B78" s="19" t="s">
+      <c r="B79" s="19" t="s">
         <v>515</v>
       </c>
-      <c r="C78" s="2">
-        <v>1</v>
-      </c>
-      <c r="D78" s="2">
-        <v>1</v>
-      </c>
-      <c r="E78" s="4">
-        <v>1</v>
-      </c>
-      <c r="F78" s="4">
-        <v>1</v>
-      </c>
-      <c r="G78" s="3">
-        <v>1</v>
-      </c>
-      <c r="H78" s="11" t="s">
+      <c r="C79" s="2">
+        <v>1</v>
+      </c>
+      <c r="D79" s="2">
+        <v>1</v>
+      </c>
+      <c r="E79" s="4">
+        <v>1</v>
+      </c>
+      <c r="F79" s="4">
+        <v>1</v>
+      </c>
+      <c r="G79" s="3">
+        <v>1</v>
+      </c>
+      <c r="H79" s="11" t="s">
         <v>515</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="11" t="s">
-        <v>509</v>
-      </c>
-      <c r="B79" s="11" t="s">
-        <v>511</v>
-      </c>
-      <c r="C79" s="2">
-        <v>1</v>
-      </c>
-      <c r="D79" s="2">
-        <v>1</v>
-      </c>
-      <c r="E79" s="4">
-        <v>1</v>
-      </c>
-      <c r="F79" s="4">
-        <v>0</v>
-      </c>
-      <c r="G79" s="3">
-        <v>1</v>
-      </c>
-      <c r="H79" s="11" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="11" t="s">
-        <v>669</v>
+        <v>509</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>670</v>
+        <v>511</v>
       </c>
       <c r="C80" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80" s="2">
         <v>1</v>
@@ -4601,432 +4613,432 @@
       <c r="H80" s="11" t="s">
         <v>510</v>
       </c>
-      <c r="I80" s="3" t="s">
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="11" t="s">
+        <v>669</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>670</v>
+      </c>
+      <c r="C81" s="2">
+        <v>0</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1</v>
+      </c>
+      <c r="E81" s="4">
+        <v>1</v>
+      </c>
+      <c r="F81" s="4">
+        <v>0</v>
+      </c>
+      <c r="G81" s="3">
+        <v>1</v>
+      </c>
+      <c r="H81" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="I81" s="3" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A81" s="11" t="s">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="11" t="s">
         <v>561</v>
       </c>
-      <c r="B81" s="11" t="s">
+      <c r="B82" s="11" t="s">
         <v>562</v>
       </c>
-      <c r="C81" s="2">
-        <v>1</v>
-      </c>
-      <c r="D81" s="2">
-        <v>1</v>
-      </c>
-      <c r="E81" s="4">
-        <v>1</v>
-      </c>
-      <c r="F81" s="4">
-        <v>0</v>
-      </c>
-      <c r="G81" s="3">
-        <v>1</v>
-      </c>
-      <c r="H81" s="11" t="s">
+      <c r="C82" s="2">
+        <v>1</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
+      <c r="E82" s="4">
+        <v>1</v>
+      </c>
+      <c r="F82" s="4">
+        <v>0</v>
+      </c>
+      <c r="G82" s="3">
+        <v>1</v>
+      </c>
+      <c r="H82" s="11" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A82" s="11" t="s">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" s="11" t="s">
         <v>564</v>
       </c>
-      <c r="B82" s="11" t="s">
+      <c r="B83" s="11" t="s">
         <v>566</v>
       </c>
-      <c r="C82" s="2">
-        <v>1</v>
-      </c>
-      <c r="D82" s="2">
-        <v>1</v>
-      </c>
-      <c r="E82" s="4">
-        <v>1</v>
-      </c>
-      <c r="F82" s="4">
-        <v>0</v>
-      </c>
-      <c r="G82" s="3">
-        <v>1</v>
-      </c>
-      <c r="H82" s="11" t="s">
+      <c r="C83" s="2">
+        <v>1</v>
+      </c>
+      <c r="D83" s="2">
+        <v>1</v>
+      </c>
+      <c r="E83" s="4">
+        <v>1</v>
+      </c>
+      <c r="F83" s="4">
+        <v>0</v>
+      </c>
+      <c r="G83" s="3">
+        <v>1</v>
+      </c>
+      <c r="H83" s="11" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A83" s="11" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" s="11" t="s">
         <v>565</v>
       </c>
-      <c r="B83" s="11" t="s">
+      <c r="B84" s="11" t="s">
         <v>567</v>
       </c>
-      <c r="C83" s="2">
-        <v>1</v>
-      </c>
-      <c r="D83" s="2">
-        <v>1</v>
-      </c>
-      <c r="E83" s="4">
-        <v>1</v>
-      </c>
-      <c r="F83" s="4">
-        <v>0</v>
-      </c>
-      <c r="G83" s="3">
-        <v>1</v>
-      </c>
-      <c r="H83" s="11" t="s">
+      <c r="C84" s="2">
+        <v>1</v>
+      </c>
+      <c r="D84" s="2">
+        <v>1</v>
+      </c>
+      <c r="E84" s="4">
+        <v>1</v>
+      </c>
+      <c r="F84" s="4">
+        <v>0</v>
+      </c>
+      <c r="G84" s="3">
+        <v>1</v>
+      </c>
+      <c r="H84" s="11" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A84" s="13" t="s">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" s="13" t="s">
         <v>377</v>
       </c>
-      <c r="B84" s="13" t="s">
+      <c r="B85" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C84" s="2">
-        <v>0</v>
-      </c>
-      <c r="D84" s="2">
-        <v>0</v>
-      </c>
-      <c r="E84" s="4">
-        <v>1</v>
-      </c>
-      <c r="F84" s="3">
-        <v>0</v>
-      </c>
-      <c r="G84" s="3">
-        <v>1</v>
-      </c>
-      <c r="H84" s="13" t="s">
+      <c r="C85" s="2">
+        <v>0</v>
+      </c>
+      <c r="D85" s="2">
+        <v>0</v>
+      </c>
+      <c r="E85" s="4">
+        <v>1</v>
+      </c>
+      <c r="F85" s="3">
+        <v>0</v>
+      </c>
+      <c r="G85" s="3">
+        <v>1</v>
+      </c>
+      <c r="H85" s="13" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A85" s="13" t="s">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" s="13" t="s">
         <v>378</v>
       </c>
-      <c r="B85" s="13" t="s">
+      <c r="B86" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C85" s="20">
-        <v>0</v>
-      </c>
-      <c r="D85" s="20">
-        <v>0</v>
-      </c>
-      <c r="E85" s="21">
-        <v>1</v>
-      </c>
-      <c r="F85" s="3">
-        <v>0</v>
-      </c>
-      <c r="G85" s="3">
-        <v>1</v>
-      </c>
-      <c r="H85" s="13" t="s">
+      <c r="C86" s="20">
+        <v>0</v>
+      </c>
+      <c r="D86" s="20">
+        <v>0</v>
+      </c>
+      <c r="E86" s="21">
+        <v>1</v>
+      </c>
+      <c r="F86" s="3">
+        <v>0</v>
+      </c>
+      <c r="G86" s="3">
+        <v>1</v>
+      </c>
+      <c r="H86" s="13" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A86" s="13" t="s">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="13" t="s">
         <v>379</v>
       </c>
-      <c r="B86" s="13" t="s">
+      <c r="B87" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C86" s="20">
-        <v>0</v>
-      </c>
-      <c r="D86" s="20">
-        <v>0</v>
-      </c>
-      <c r="E86" s="20">
-        <v>1</v>
-      </c>
-      <c r="F86" s="3">
-        <v>0</v>
-      </c>
-      <c r="G86" s="3">
-        <v>1</v>
-      </c>
-      <c r="H86" s="13" t="s">
+      <c r="C87" s="20">
+        <v>0</v>
+      </c>
+      <c r="D87" s="20">
+        <v>0</v>
+      </c>
+      <c r="E87" s="20">
+        <v>1</v>
+      </c>
+      <c r="F87" s="3">
+        <v>0</v>
+      </c>
+      <c r="G87" s="3">
+        <v>1</v>
+      </c>
+      <c r="H87" s="13" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A87" s="13" t="s">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="13" t="s">
         <v>380</v>
       </c>
-      <c r="B87" s="13" t="s">
+      <c r="B88" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C87" s="20">
-        <v>0</v>
-      </c>
-      <c r="D87" s="20">
-        <v>0</v>
-      </c>
-      <c r="E87" s="21">
-        <v>1</v>
-      </c>
-      <c r="F87" s="3">
-        <v>0</v>
-      </c>
-      <c r="G87" s="3">
-        <v>1</v>
-      </c>
-      <c r="H87" s="13" t="s">
+      <c r="C88" s="20">
+        <v>0</v>
+      </c>
+      <c r="D88" s="20">
+        <v>0</v>
+      </c>
+      <c r="E88" s="21">
+        <v>1</v>
+      </c>
+      <c r="F88" s="3">
+        <v>0</v>
+      </c>
+      <c r="G88" s="3">
+        <v>1</v>
+      </c>
+      <c r="H88" s="13" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A88" s="13" t="s">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" s="13" t="s">
         <v>381</v>
       </c>
-      <c r="B88" s="13" t="s">
+      <c r="B89" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C88" s="20">
-        <v>0</v>
-      </c>
-      <c r="D88" s="20">
-        <v>0</v>
-      </c>
-      <c r="E88" s="21">
-        <v>1</v>
-      </c>
-      <c r="F88" s="3">
-        <v>0</v>
-      </c>
-      <c r="G88" s="3">
-        <v>1</v>
-      </c>
-      <c r="H88" s="13" t="s">
+      <c r="C89" s="20">
+        <v>0</v>
+      </c>
+      <c r="D89" s="20">
+        <v>0</v>
+      </c>
+      <c r="E89" s="21">
+        <v>1</v>
+      </c>
+      <c r="F89" s="3">
+        <v>0</v>
+      </c>
+      <c r="G89" s="3">
+        <v>1</v>
+      </c>
+      <c r="H89" s="13" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A89" s="13" t="s">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="13" t="s">
         <v>382</v>
       </c>
-      <c r="B89" s="13" t="s">
+      <c r="B90" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C89" s="2">
-        <v>0</v>
-      </c>
-      <c r="D89" s="2">
-        <v>0</v>
-      </c>
-      <c r="E89" s="4">
-        <v>1</v>
-      </c>
-      <c r="F89" s="3">
-        <v>0</v>
-      </c>
-      <c r="G89" s="3">
-        <v>1</v>
-      </c>
-      <c r="H89" s="13" t="s">
+      <c r="C90" s="2">
+        <v>0</v>
+      </c>
+      <c r="D90" s="2">
+        <v>0</v>
+      </c>
+      <c r="E90" s="4">
+        <v>1</v>
+      </c>
+      <c r="F90" s="3">
+        <v>0</v>
+      </c>
+      <c r="G90" s="3">
+        <v>1</v>
+      </c>
+      <c r="H90" s="13" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A90" s="13" t="s">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" s="13" t="s">
         <v>383</v>
       </c>
-      <c r="B90" s="13" t="s">
+      <c r="B91" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C90" s="2">
-        <v>0</v>
-      </c>
-      <c r="D90" s="2">
-        <v>0</v>
-      </c>
-      <c r="E90" s="4">
-        <v>1</v>
-      </c>
-      <c r="F90" s="3">
-        <v>0</v>
-      </c>
-      <c r="G90" s="3">
-        <v>1</v>
-      </c>
-      <c r="H90" s="13" t="s">
+      <c r="C91" s="2">
+        <v>0</v>
+      </c>
+      <c r="D91" s="2">
+        <v>0</v>
+      </c>
+      <c r="E91" s="4">
+        <v>1</v>
+      </c>
+      <c r="F91" s="3">
+        <v>0</v>
+      </c>
+      <c r="G91" s="3">
+        <v>1</v>
+      </c>
+      <c r="H91" s="13" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A91" s="13" t="s">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="13" t="s">
         <v>384</v>
       </c>
-      <c r="B91" s="13" t="s">
+      <c r="B92" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C91" s="2">
-        <v>0</v>
-      </c>
-      <c r="D91" s="2">
-        <v>0</v>
-      </c>
-      <c r="E91" s="4">
-        <v>1</v>
-      </c>
-      <c r="F91" s="3">
-        <v>0</v>
-      </c>
-      <c r="G91" s="3">
-        <v>1</v>
-      </c>
-      <c r="H91" s="13" t="s">
+      <c r="C92" s="2">
+        <v>0</v>
+      </c>
+      <c r="D92" s="2">
+        <v>0</v>
+      </c>
+      <c r="E92" s="4">
+        <v>1</v>
+      </c>
+      <c r="F92" s="3">
+        <v>0</v>
+      </c>
+      <c r="G92" s="3">
+        <v>1</v>
+      </c>
+      <c r="H92" s="13" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A92" s="13" t="s">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" s="13" t="s">
         <v>385</v>
       </c>
-      <c r="B92" s="13" t="s">
+      <c r="B93" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C92" s="2">
-        <v>0</v>
-      </c>
-      <c r="D92" s="2">
-        <v>0</v>
-      </c>
-      <c r="E92" s="4">
-        <v>1</v>
-      </c>
-      <c r="F92" s="3">
-        <v>0</v>
-      </c>
-      <c r="G92" s="3">
-        <v>1</v>
-      </c>
-      <c r="H92" s="13" t="s">
+      <c r="C93" s="2">
+        <v>0</v>
+      </c>
+      <c r="D93" s="2">
+        <v>0</v>
+      </c>
+      <c r="E93" s="4">
+        <v>1</v>
+      </c>
+      <c r="F93" s="3">
+        <v>0</v>
+      </c>
+      <c r="G93" s="3">
+        <v>1</v>
+      </c>
+      <c r="H93" s="13" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A93" s="13" t="s">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A94" s="13" t="s">
         <v>386</v>
       </c>
-      <c r="B93" s="13" t="s">
+      <c r="B94" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C93" s="2">
-        <v>0</v>
-      </c>
-      <c r="D93" s="2">
-        <v>0</v>
-      </c>
-      <c r="E93" s="4">
-        <v>1</v>
-      </c>
-      <c r="F93" s="3">
-        <v>0</v>
-      </c>
-      <c r="G93" s="3">
-        <v>1</v>
-      </c>
-      <c r="H93" s="13" t="s">
+      <c r="C94" s="2">
+        <v>0</v>
+      </c>
+      <c r="D94" s="2">
+        <v>0</v>
+      </c>
+      <c r="E94" s="4">
+        <v>1</v>
+      </c>
+      <c r="F94" s="3">
+        <v>0</v>
+      </c>
+      <c r="G94" s="3">
+        <v>1</v>
+      </c>
+      <c r="H94" s="13" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A94" s="13" t="s">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A95" s="13" t="s">
         <v>387</v>
       </c>
-      <c r="B94" s="13" t="s">
+      <c r="B95" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C94" s="2">
-        <v>0</v>
-      </c>
-      <c r="D94" s="2">
-        <v>0</v>
-      </c>
-      <c r="E94" s="4">
-        <v>1</v>
-      </c>
-      <c r="F94" s="3">
-        <v>0</v>
-      </c>
-      <c r="G94" s="3">
-        <v>1</v>
-      </c>
-      <c r="H94" s="13" t="s">
+      <c r="C95" s="2">
+        <v>0</v>
+      </c>
+      <c r="D95" s="2">
+        <v>0</v>
+      </c>
+      <c r="E95" s="4">
+        <v>1</v>
+      </c>
+      <c r="F95" s="3">
+        <v>0</v>
+      </c>
+      <c r="G95" s="3">
+        <v>1</v>
+      </c>
+      <c r="H95" s="13" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A95" s="13" t="s">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A96" s="13" t="s">
         <v>388</v>
       </c>
-      <c r="B95" s="13" t="s">
+      <c r="B96" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C95" s="2">
-        <v>0</v>
-      </c>
-      <c r="D95" s="2">
-        <v>0</v>
-      </c>
-      <c r="E95" s="4">
-        <v>1</v>
-      </c>
-      <c r="F95" s="3">
-        <v>0</v>
-      </c>
-      <c r="G95" s="3">
-        <v>1</v>
-      </c>
-      <c r="H95" s="13" t="s">
+      <c r="C96" s="2">
+        <v>0</v>
+      </c>
+      <c r="D96" s="2">
+        <v>0</v>
+      </c>
+      <c r="E96" s="4">
+        <v>1</v>
+      </c>
+      <c r="F96" s="3">
+        <v>0</v>
+      </c>
+      <c r="G96" s="3">
+        <v>1</v>
+      </c>
+      <c r="H96" s="13" t="s">
         <v>240</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A96" s="13" t="s">
-        <v>389</v>
-      </c>
-      <c r="B96" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C96" s="2">
-        <v>0</v>
-      </c>
-      <c r="D96" s="2">
-        <v>0</v>
-      </c>
-      <c r="E96" s="4">
-        <v>1</v>
-      </c>
-      <c r="F96" s="3">
-        <v>0</v>
-      </c>
-      <c r="G96" s="3">
-        <v>1</v>
-      </c>
-      <c r="H96" s="13" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C97" s="2">
         <v>0</v>
@@ -5044,15 +5056,15 @@
         <v>1</v>
       </c>
       <c r="H97" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B98" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C98" s="2">
         <v>0</v>
@@ -5070,15 +5082,15 @@
         <v>1</v>
       </c>
       <c r="H98" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C99" s="2">
         <v>0</v>
@@ -5096,15 +5108,15 @@
         <v>1</v>
       </c>
       <c r="H99" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C100" s="2">
         <v>0</v>
@@ -5122,15 +5134,15 @@
         <v>1</v>
       </c>
       <c r="H100" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B101" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C101" s="2">
         <v>0</v>
@@ -5148,15 +5160,15 @@
         <v>1</v>
       </c>
       <c r="H101" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C102" s="2">
         <v>0</v>
@@ -5174,15 +5186,15 @@
         <v>1</v>
       </c>
       <c r="H102" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C103" s="2">
         <v>0</v>
@@ -5200,23 +5212,23 @@
         <v>1</v>
       </c>
       <c r="H103" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C104" s="20">
+        <v>70</v>
+      </c>
+      <c r="C104" s="2">
         <v>0</v>
       </c>
       <c r="D104" s="2">
         <v>0</v>
       </c>
-      <c r="E104" s="21">
+      <c r="E104" s="4">
         <v>1</v>
       </c>
       <c r="F104" s="3">
@@ -5226,15 +5238,15 @@
         <v>1</v>
       </c>
       <c r="H104" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C105" s="20">
         <v>0</v>
@@ -5242,7 +5254,7 @@
       <c r="D105" s="2">
         <v>0</v>
       </c>
-      <c r="E105" s="20">
+      <c r="E105" s="21">
         <v>1</v>
       </c>
       <c r="F105" s="3">
@@ -5252,15 +5264,15 @@
         <v>1</v>
       </c>
       <c r="H105" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C106" s="20">
         <v>0</v>
@@ -5268,7 +5280,7 @@
       <c r="D106" s="2">
         <v>0</v>
       </c>
-      <c r="E106" s="21">
+      <c r="E106" s="20">
         <v>1</v>
       </c>
       <c r="F106" s="3">
@@ -5278,15 +5290,15 @@
         <v>1</v>
       </c>
       <c r="H106" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="13" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C107" s="20">
         <v>0</v>
@@ -5304,15 +5316,15 @@
         <v>1</v>
       </c>
       <c r="H107" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C108" s="20">
         <v>0</v>
@@ -5320,7 +5332,7 @@
       <c r="D108" s="2">
         <v>0</v>
       </c>
-      <c r="E108" s="20">
+      <c r="E108" s="21">
         <v>1</v>
       </c>
       <c r="F108" s="3">
@@ -5330,15 +5342,15 @@
         <v>1</v>
       </c>
       <c r="H108" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C109" s="20">
         <v>0</v>
@@ -5346,7 +5358,7 @@
       <c r="D109" s="2">
         <v>0</v>
       </c>
-      <c r="E109" s="4">
+      <c r="E109" s="20">
         <v>1</v>
       </c>
       <c r="F109" s="3">
@@ -5356,15 +5368,15 @@
         <v>1</v>
       </c>
       <c r="H109" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="13" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C110" s="20">
         <v>0</v>
@@ -5382,17 +5394,17 @@
         <v>1</v>
       </c>
       <c r="H110" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B111" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C111" s="2">
+        <v>77</v>
+      </c>
+      <c r="C111" s="20">
         <v>0</v>
       </c>
       <c r="D111" s="2">
@@ -5408,67 +5420,67 @@
         <v>1</v>
       </c>
       <c r="H111" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="13" t="s">
+        <v>404</v>
+      </c>
+      <c r="B112" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C112" s="2">
+        <v>0</v>
+      </c>
+      <c r="D112" s="2">
+        <v>0</v>
+      </c>
+      <c r="E112" s="4">
+        <v>1</v>
+      </c>
+      <c r="F112" s="3">
+        <v>0</v>
+      </c>
+      <c r="G112" s="3">
+        <v>1</v>
+      </c>
+      <c r="H112" s="13" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A113" s="13" t="s">
         <v>405</v>
       </c>
-      <c r="B112" s="13" t="s">
+      <c r="B113" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C112" s="2">
-        <v>0</v>
-      </c>
-      <c r="D112" s="2">
-        <v>0</v>
-      </c>
-      <c r="E112" s="4">
-        <v>1</v>
-      </c>
-      <c r="F112" s="3">
-        <v>0</v>
-      </c>
-      <c r="G112" s="3">
-        <v>1</v>
-      </c>
-      <c r="H112" s="13" t="s">
+      <c r="C113" s="2">
+        <v>0</v>
+      </c>
+      <c r="D113" s="2">
+        <v>0</v>
+      </c>
+      <c r="E113" s="4">
+        <v>1</v>
+      </c>
+      <c r="F113" s="3">
+        <v>0</v>
+      </c>
+      <c r="G113" s="3">
+        <v>1</v>
+      </c>
+      <c r="H113" s="13" t="s">
         <v>257</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A113" s="17" t="s">
-        <v>406</v>
-      </c>
-      <c r="B113" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C113" s="2">
-        <v>0</v>
-      </c>
-      <c r="D113" s="2">
-        <v>0</v>
-      </c>
-      <c r="E113" s="2">
-        <v>1</v>
-      </c>
-      <c r="F113" s="3">
-        <v>1</v>
-      </c>
-      <c r="G113" s="3">
-        <v>1</v>
-      </c>
-      <c r="H113" s="17" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="17" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C114" s="2">
         <v>0</v>
@@ -5483,18 +5495,18 @@
         <v>1</v>
       </c>
       <c r="G114" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H114" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="17" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C115" s="2">
         <v>0</v>
@@ -5512,15 +5524,15 @@
         <v>0</v>
       </c>
       <c r="H115" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="17" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C116" s="2">
         <v>0</v>
@@ -5538,15 +5550,15 @@
         <v>0</v>
       </c>
       <c r="H116" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="17" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C117" s="2">
         <v>0</v>
@@ -5564,15 +5576,15 @@
         <v>0</v>
       </c>
       <c r="H117" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="17" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C118" s="2">
         <v>0</v>
@@ -5590,15 +5602,15 @@
         <v>0</v>
       </c>
       <c r="H118" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="17" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C119" s="2">
         <v>0</v>
@@ -5616,15 +5628,15 @@
         <v>0</v>
       </c>
       <c r="H119" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="17" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B120" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C120" s="2">
         <v>0</v>
@@ -5642,15 +5654,15 @@
         <v>0</v>
       </c>
       <c r="H120" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="17" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C121" s="2">
         <v>0</v>
@@ -5668,15 +5680,15 @@
         <v>0</v>
       </c>
       <c r="H121" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="17" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B122" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C122" s="2">
         <v>0</v>
@@ -5694,15 +5706,15 @@
         <v>0</v>
       </c>
       <c r="H122" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B123" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C123" s="2">
         <v>0</v>
@@ -5720,15 +5732,15 @@
         <v>0</v>
       </c>
       <c r="H123" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="17" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B124" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C124" s="2">
         <v>0</v>
@@ -5746,15 +5758,15 @@
         <v>0</v>
       </c>
       <c r="H124" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="17" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B125" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C125" s="2">
         <v>0</v>
@@ -5772,15 +5784,15 @@
         <v>0</v>
       </c>
       <c r="H125" s="17" t="s">
-        <v>258</v>
+        <v>236</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B126" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C126" s="2">
         <v>0</v>
@@ -5798,15 +5810,15 @@
         <v>0</v>
       </c>
       <c r="H126" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B127" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C127" s="2">
         <v>0</v>
@@ -5824,15 +5836,15 @@
         <v>0</v>
       </c>
       <c r="H127" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="17" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C128" s="2">
         <v>0</v>
@@ -5850,15 +5862,15 @@
         <v>0</v>
       </c>
       <c r="H128" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="17" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C129" s="2">
         <v>0</v>
@@ -5876,15 +5888,15 @@
         <v>0</v>
       </c>
       <c r="H129" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="17" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C130" s="2">
         <v>0</v>
@@ -5899,18 +5911,18 @@
         <v>1</v>
       </c>
       <c r="G130" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H130" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="17" t="s">
-        <v>424</v>
-      </c>
-      <c r="B131" s="15" t="s">
-        <v>98</v>
+        <v>423</v>
+      </c>
+      <c r="B131" s="14" t="s">
+        <v>97</v>
       </c>
       <c r="C131" s="2">
         <v>0</v>
@@ -5928,15 +5940,15 @@
         <v>1</v>
       </c>
       <c r="H131" s="17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="17" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B132" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C132" s="2">
         <v>0</v>
@@ -5954,15 +5966,15 @@
         <v>1</v>
       </c>
       <c r="H132" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="17" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B133" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C133" s="2">
         <v>0</v>
@@ -5980,15 +5992,15 @@
         <v>1</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="17" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B134" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C134" s="2">
         <v>0</v>
@@ -6006,15 +6018,15 @@
         <v>1</v>
       </c>
       <c r="H134" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="17" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B135" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C135" s="2">
         <v>0</v>
@@ -6032,15 +6044,15 @@
         <v>1</v>
       </c>
       <c r="H135" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="17" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B136" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C136" s="2">
         <v>0</v>
@@ -6058,15 +6070,15 @@
         <v>1</v>
       </c>
       <c r="H136" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="17" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B137" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C137" s="2">
         <v>0</v>
@@ -6084,15 +6096,15 @@
         <v>1</v>
       </c>
       <c r="H137" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B138" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C138" s="2">
         <v>0</v>
@@ -6100,25 +6112,25 @@
       <c r="D138" s="2">
         <v>0</v>
       </c>
-      <c r="E138" s="20">
-        <v>1</v>
-      </c>
-      <c r="F138" s="22">
+      <c r="E138" s="2">
+        <v>1</v>
+      </c>
+      <c r="F138" s="3">
         <v>1</v>
       </c>
       <c r="G138" s="3">
         <v>1</v>
       </c>
       <c r="H138" s="17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="17" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B139" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C139" s="2">
         <v>0</v>
@@ -6136,15 +6148,15 @@
         <v>1</v>
       </c>
       <c r="H139" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B140" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C140" s="2">
         <v>0</v>
@@ -6162,15 +6174,15 @@
         <v>1</v>
       </c>
       <c r="H140" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="17" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B141" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C141" s="2">
         <v>0</v>
@@ -6181,22 +6193,22 @@
       <c r="E141" s="20">
         <v>1</v>
       </c>
-      <c r="F141" s="20">
+      <c r="F141" s="22">
         <v>1</v>
       </c>
       <c r="G141" s="3">
         <v>1</v>
       </c>
       <c r="H141" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="17" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B142" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C142" s="2">
         <v>0</v>
@@ -6207,22 +6219,22 @@
       <c r="E142" s="20">
         <v>1</v>
       </c>
-      <c r="F142" s="22">
+      <c r="F142" s="20">
         <v>1</v>
       </c>
       <c r="G142" s="3">
         <v>1</v>
       </c>
       <c r="H142" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="17" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B143" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C143" s="2">
         <v>0</v>
@@ -6240,15 +6252,15 @@
         <v>1</v>
       </c>
       <c r="H143" s="17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="17" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B144" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C144" s="2">
         <v>0</v>
@@ -6266,15 +6278,15 @@
         <v>1</v>
       </c>
       <c r="H144" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" s="17" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B145" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C145" s="2">
         <v>0</v>
@@ -6285,22 +6297,22 @@
       <c r="E145" s="20">
         <v>1</v>
       </c>
-      <c r="F145" s="20">
+      <c r="F145" s="22">
         <v>1</v>
       </c>
       <c r="G145" s="3">
         <v>1</v>
       </c>
       <c r="H145" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="17" t="s">
-        <v>439</v>
-      </c>
-      <c r="B146" s="14" t="s">
-        <v>113</v>
+        <v>438</v>
+      </c>
+      <c r="B146" s="15" t="s">
+        <v>112</v>
       </c>
       <c r="C146" s="2">
         <v>0</v>
@@ -6311,22 +6323,22 @@
       <c r="E146" s="20">
         <v>1</v>
       </c>
-      <c r="F146" s="22">
+      <c r="F146" s="20">
         <v>1</v>
       </c>
       <c r="G146" s="3">
         <v>1</v>
       </c>
       <c r="H146" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="17" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B147" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C147" s="2">
         <v>0</v>
@@ -6341,18 +6353,18 @@
         <v>1</v>
       </c>
       <c r="G147" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H147" s="17" t="s">
-        <v>114</v>
+        <v>279</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="17" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B148" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C148" s="2">
         <v>0</v>
@@ -6370,15 +6382,15 @@
         <v>0</v>
       </c>
       <c r="H148" s="17" t="s">
-        <v>280</v>
+        <v>114</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" s="17" t="s">
-        <v>609</v>
+        <v>441</v>
       </c>
       <c r="B149" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C149" s="2">
         <v>0</v>
@@ -6396,15 +6408,15 @@
         <v>0</v>
       </c>
       <c r="H149" s="17" t="s">
-        <v>612</v>
+        <v>280</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="17" t="s">
-        <v>442</v>
+        <v>609</v>
       </c>
       <c r="B150" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C150" s="2">
         <v>0</v>
@@ -6422,15 +6434,15 @@
         <v>0</v>
       </c>
       <c r="H150" s="17" t="s">
-        <v>281</v>
+        <v>612</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="17" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B151" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C151" s="2">
         <v>0</v>
@@ -6441,22 +6453,22 @@
       <c r="E151" s="20">
         <v>1</v>
       </c>
-      <c r="F151" s="20">
+      <c r="F151" s="22">
         <v>1</v>
       </c>
       <c r="G151" s="3">
         <v>0</v>
       </c>
       <c r="H151" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" s="17" t="s">
-        <v>620</v>
+        <v>443</v>
       </c>
       <c r="B152" s="14" t="s">
-        <v>610</v>
+        <v>118</v>
       </c>
       <c r="C152" s="2">
         <v>0</v>
@@ -6467,22 +6479,22 @@
       <c r="E152" s="20">
         <v>1</v>
       </c>
-      <c r="F152" s="22">
+      <c r="F152" s="20">
         <v>1</v>
       </c>
       <c r="G152" s="3">
         <v>0</v>
       </c>
       <c r="H152" s="17" t="s">
-        <v>611</v>
+        <v>282</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" s="17" t="s">
-        <v>444</v>
+        <v>620</v>
       </c>
       <c r="B153" s="14" t="s">
-        <v>119</v>
+        <v>610</v>
       </c>
       <c r="C153" s="2">
         <v>0</v>
@@ -6500,15 +6512,15 @@
         <v>0</v>
       </c>
       <c r="H153" s="17" t="s">
-        <v>283</v>
+        <v>611</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" s="17" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B154" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C154" s="2">
         <v>0</v>
@@ -6526,67 +6538,67 @@
         <v>0</v>
       </c>
       <c r="H154" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" s="17" t="s">
+        <v>445</v>
+      </c>
+      <c r="B155" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C155" s="2">
+        <v>0</v>
+      </c>
+      <c r="D155" s="2">
+        <v>0</v>
+      </c>
+      <c r="E155" s="20">
+        <v>1</v>
+      </c>
+      <c r="F155" s="22">
+        <v>1</v>
+      </c>
+      <c r="G155" s="3">
+        <v>0</v>
+      </c>
+      <c r="H155" s="17" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A156" s="17" t="s">
         <v>446</v>
       </c>
-      <c r="B155" s="14" t="s">
+      <c r="B156" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C155" s="2">
-        <v>0</v>
-      </c>
-      <c r="D155" s="2">
-        <v>0</v>
-      </c>
-      <c r="E155" s="20">
-        <v>1</v>
-      </c>
-      <c r="F155" s="22">
-        <v>1</v>
-      </c>
-      <c r="G155" s="3">
-        <v>0</v>
-      </c>
-      <c r="H155" s="17" t="s">
+      <c r="C156" s="2">
+        <v>0</v>
+      </c>
+      <c r="D156" s="2">
+        <v>0</v>
+      </c>
+      <c r="E156" s="20">
+        <v>1</v>
+      </c>
+      <c r="F156" s="22">
+        <v>1</v>
+      </c>
+      <c r="G156" s="3">
+        <v>0</v>
+      </c>
+      <c r="H156" s="17" t="s">
         <v>285</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A156" s="18" t="s">
-        <v>597</v>
-      </c>
-      <c r="B156" s="16" t="s">
-        <v>603</v>
-      </c>
-      <c r="C156" s="2">
-        <v>0</v>
-      </c>
-      <c r="D156" s="2">
-        <v>0</v>
-      </c>
-      <c r="E156" s="20">
-        <v>1</v>
-      </c>
-      <c r="F156" s="20">
-        <v>1</v>
-      </c>
-      <c r="G156" s="3">
-        <v>0</v>
-      </c>
-      <c r="H156" s="18" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" s="18" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B157" s="16" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C157" s="2">
         <v>0</v>
@@ -6604,15 +6616,15 @@
         <v>0</v>
       </c>
       <c r="H157" s="18" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" s="18" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B158" s="16" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C158" s="2">
         <v>0</v>
@@ -6630,15 +6642,15 @@
         <v>0</v>
       </c>
       <c r="H158" s="18" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" s="18" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B159" s="16" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C159" s="2">
         <v>0</v>
@@ -6656,15 +6668,15 @@
         <v>0</v>
       </c>
       <c r="H159" s="18" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" s="18" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B160" s="16" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C160" s="2">
         <v>0</v>
@@ -6682,122 +6694,122 @@
         <v>0</v>
       </c>
       <c r="H160" s="18" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" s="18" t="s">
+        <v>601</v>
+      </c>
+      <c r="B161" s="16" t="s">
+        <v>607</v>
+      </c>
+      <c r="C161" s="2">
+        <v>0</v>
+      </c>
+      <c r="D161" s="2">
+        <v>0</v>
+      </c>
+      <c r="E161" s="20">
+        <v>1</v>
+      </c>
+      <c r="F161" s="20">
+        <v>1</v>
+      </c>
+      <c r="G161" s="3">
+        <v>0</v>
+      </c>
+      <c r="H161" s="18" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A162" s="18" t="s">
         <v>602</v>
       </c>
-      <c r="B161" s="16" t="s">
+      <c r="B162" s="16" t="s">
         <v>608</v>
       </c>
-      <c r="C161" s="2">
-        <v>0</v>
-      </c>
-      <c r="D161" s="2">
-        <v>0</v>
-      </c>
-      <c r="E161" s="20">
-        <v>1</v>
-      </c>
-      <c r="F161" s="20">
-        <v>1</v>
-      </c>
-      <c r="G161" s="3">
-        <v>0</v>
-      </c>
-      <c r="H161" s="18" t="s">
+      <c r="C162" s="2">
+        <v>0</v>
+      </c>
+      <c r="D162" s="2">
+        <v>0</v>
+      </c>
+      <c r="E162" s="20">
+        <v>1</v>
+      </c>
+      <c r="F162" s="20">
+        <v>1</v>
+      </c>
+      <c r="G162" s="3">
+        <v>0</v>
+      </c>
+      <c r="H162" s="18" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A162" s="17" t="s">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A163" s="17" t="s">
         <v>619</v>
       </c>
-      <c r="B162" s="14" t="s">
+      <c r="B163" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C162" s="2">
-        <v>0</v>
-      </c>
-      <c r="D162" s="2">
-        <v>0</v>
-      </c>
-      <c r="E162" s="20">
-        <v>1</v>
-      </c>
-      <c r="F162" s="22">
-        <v>1</v>
-      </c>
-      <c r="G162" s="3">
-        <v>0</v>
-      </c>
-      <c r="H162" s="17" t="s">
+      <c r="C163" s="2">
+        <v>0</v>
+      </c>
+      <c r="D163" s="2">
+        <v>0</v>
+      </c>
+      <c r="E163" s="20">
+        <v>1</v>
+      </c>
+      <c r="F163" s="22">
+        <v>1</v>
+      </c>
+      <c r="G163" s="3">
+        <v>0</v>
+      </c>
+      <c r="H163" s="17" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A163" s="26" t="s">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A164" s="26" t="s">
         <v>671</v>
       </c>
-      <c r="B163" s="28" t="s">
+      <c r="B164" s="28" t="s">
         <v>672</v>
       </c>
-      <c r="C163" s="2">
-        <v>0</v>
-      </c>
-      <c r="D163" s="2">
-        <v>1</v>
-      </c>
-      <c r="E163" s="4">
-        <v>1</v>
-      </c>
-      <c r="F163" s="3">
-        <v>1</v>
-      </c>
-      <c r="G163" s="3">
-        <v>0</v>
-      </c>
-      <c r="H163" s="27" t="s">
+      <c r="C164" s="2">
+        <v>0</v>
+      </c>
+      <c r="D164" s="2">
+        <v>1</v>
+      </c>
+      <c r="E164" s="4">
+        <v>1</v>
+      </c>
+      <c r="F164" s="3">
+        <v>1</v>
+      </c>
+      <c r="G164" s="3">
+        <v>0</v>
+      </c>
+      <c r="H164" s="27" t="s">
         <v>673</v>
       </c>
-      <c r="I163" s="3" t="s">
+      <c r="I164" s="3" t="s">
         <v>658</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A164" s="17" t="s">
-        <v>579</v>
-      </c>
-      <c r="B164" s="23" t="s">
-        <v>541</v>
-      </c>
-      <c r="C164" s="2">
-        <v>0</v>
-      </c>
-      <c r="D164" s="2">
-        <v>0</v>
-      </c>
-      <c r="E164" s="4">
-        <v>1</v>
-      </c>
-      <c r="F164" s="22">
-        <v>1</v>
-      </c>
-      <c r="G164" s="3">
-        <v>0</v>
-      </c>
-      <c r="H164" s="17" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" s="17" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B165" s="23" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C165" s="2">
         <v>0</v>
@@ -6815,15 +6827,15 @@
         <v>0</v>
       </c>
       <c r="H165" s="17" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" s="17" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B166" s="23" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="C166" s="2">
         <v>0</v>
@@ -6841,15 +6853,15 @@
         <v>0</v>
       </c>
       <c r="H166" s="17" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" s="17" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B167" s="23" t="s">
-        <v>543</v>
+        <v>548</v>
       </c>
       <c r="C167" s="2">
         <v>0</v>
@@ -6867,15 +6879,15 @@
         <v>0</v>
       </c>
       <c r="H167" s="17" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" s="17" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B168" s="23" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="C168" s="2">
         <v>0</v>
@@ -6893,15 +6905,15 @@
         <v>0</v>
       </c>
       <c r="H168" s="17" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" s="17" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B169" s="23" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C169" s="2">
         <v>0</v>
@@ -6919,15 +6931,15 @@
         <v>0</v>
       </c>
       <c r="H169" s="17" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" s="17" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B170" s="23" t="s">
-        <v>544</v>
+        <v>550</v>
       </c>
       <c r="C170" s="2">
         <v>0</v>
@@ -6945,15 +6957,15 @@
         <v>0</v>
       </c>
       <c r="H170" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" s="17" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B171" s="23" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="C171" s="2">
         <v>0</v>
@@ -6971,15 +6983,15 @@
         <v>0</v>
       </c>
       <c r="H171" s="17" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" s="17" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B172" s="23" t="s">
-        <v>545</v>
+        <v>551</v>
       </c>
       <c r="C172" s="2">
         <v>0</v>
@@ -6997,15 +7009,15 @@
         <v>0</v>
       </c>
       <c r="H172" s="17" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" s="17" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B173" s="23" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="C173" s="2">
         <v>0</v>
@@ -7023,15 +7035,15 @@
         <v>0</v>
       </c>
       <c r="H173" s="17" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" s="17" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B174" s="23" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C174" s="2">
         <v>0</v>
@@ -7049,15 +7061,15 @@
         <v>0</v>
       </c>
       <c r="H174" s="17" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" s="17" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B175" s="23" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C175" s="2">
         <v>0</v>
@@ -7075,15 +7087,15 @@
         <v>0</v>
       </c>
       <c r="H175" s="17" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" s="17" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B176" s="23" t="s">
-        <v>546</v>
+        <v>554</v>
       </c>
       <c r="C176" s="2">
         <v>0</v>
@@ -7101,15 +7113,15 @@
         <v>0</v>
       </c>
       <c r="H176" s="17" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" s="17" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B177" s="23" t="s">
-        <v>555</v>
+        <v>546</v>
       </c>
       <c r="C177" s="2">
         <v>0</v>
@@ -7127,15 +7139,15 @@
         <v>0</v>
       </c>
       <c r="H177" s="17" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" s="17" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B178" s="23" t="s">
-        <v>547</v>
+        <v>555</v>
       </c>
       <c r="C178" s="2">
         <v>0</v>
@@ -7153,15 +7165,15 @@
         <v>0</v>
       </c>
       <c r="H178" s="17" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" s="17" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B179" s="23" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
       <c r="C179" s="2">
         <v>0</v>
@@ -7179,15 +7191,15 @@
         <v>0</v>
       </c>
       <c r="H179" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" s="17" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B180" s="23" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C180" s="2">
         <v>0</v>
@@ -7205,15 +7217,15 @@
         <v>0</v>
       </c>
       <c r="H180" s="17" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" s="17" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B181" s="23" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C181" s="2">
         <v>0</v>
@@ -7231,15 +7243,15 @@
         <v>0</v>
       </c>
       <c r="H181" s="17" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" s="17" t="s">
-        <v>447</v>
-      </c>
-      <c r="B182" s="14" t="s">
-        <v>123</v>
+        <v>596</v>
+      </c>
+      <c r="B182" s="23" t="s">
+        <v>557</v>
       </c>
       <c r="C182" s="2">
         <v>0</v>
@@ -7247,7 +7259,7 @@
       <c r="D182" s="2">
         <v>0</v>
       </c>
-      <c r="E182" s="20">
+      <c r="E182" s="4">
         <v>1</v>
       </c>
       <c r="F182" s="22">
@@ -7257,15 +7269,15 @@
         <v>0</v>
       </c>
       <c r="H182" s="17" t="s">
-        <v>287</v>
+        <v>540</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" s="17" t="s">
-        <v>559</v>
+        <v>447</v>
       </c>
       <c r="B183" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C183" s="2">
         <v>0</v>
@@ -7283,15 +7295,15 @@
         <v>0</v>
       </c>
       <c r="H183" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" s="17" t="s">
-        <v>448</v>
+        <v>559</v>
       </c>
       <c r="B184" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C184" s="2">
         <v>0</v>
@@ -7306,18 +7318,18 @@
         <v>1</v>
       </c>
       <c r="G184" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H184" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" s="17" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B185" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C185" s="2">
         <v>0</v>
@@ -7335,15 +7347,15 @@
         <v>1</v>
       </c>
       <c r="H185" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" s="17" t="s">
-        <v>573</v>
+        <v>449</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>574</v>
+        <v>126</v>
       </c>
       <c r="C186" s="2">
         <v>0</v>
@@ -7361,15 +7373,15 @@
         <v>1</v>
       </c>
       <c r="H186" s="17" t="s">
-        <v>575</v>
+        <v>290</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" s="17" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B187" s="14" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C187" s="2">
         <v>0</v>
@@ -7387,15 +7399,15 @@
         <v>1</v>
       </c>
       <c r="H187" s="17" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" s="17" t="s">
-        <v>450</v>
-      </c>
-      <c r="B188" s="15" t="s">
-        <v>127</v>
+        <v>576</v>
+      </c>
+      <c r="B188" s="14" t="s">
+        <v>577</v>
       </c>
       <c r="C188" s="2">
         <v>0</v>
@@ -7410,18 +7422,18 @@
         <v>1</v>
       </c>
       <c r="G188" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H188" s="17" t="s">
-        <v>291</v>
+        <v>578</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B189" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C189" s="2">
         <v>0</v>
@@ -7439,15 +7451,15 @@
         <v>0</v>
       </c>
       <c r="H189" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" s="17" t="s">
-        <v>452</v>
-      </c>
-      <c r="B190" s="14" t="s">
-        <v>129</v>
+        <v>451</v>
+      </c>
+      <c r="B190" s="15" t="s">
+        <v>128</v>
       </c>
       <c r="C190" s="2">
         <v>0</v>
@@ -7465,15 +7477,15 @@
         <v>0</v>
       </c>
       <c r="H190" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" s="17" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B191" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C191" s="2">
         <v>0</v>
@@ -7484,22 +7496,22 @@
       <c r="E191" s="20">
         <v>1</v>
       </c>
-      <c r="F191" s="20">
+      <c r="F191" s="22">
         <v>1</v>
       </c>
       <c r="G191" s="3">
         <v>0</v>
       </c>
       <c r="H191" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" s="17" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B192" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C192" s="2">
         <v>0</v>
@@ -7510,22 +7522,22 @@
       <c r="E192" s="20">
         <v>1</v>
       </c>
-      <c r="F192" s="22">
+      <c r="F192" s="20">
         <v>1</v>
       </c>
       <c r="G192" s="3">
         <v>0</v>
       </c>
       <c r="H192" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" s="17" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B193" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C193" s="2">
         <v>0</v>
@@ -7543,15 +7555,15 @@
         <v>0</v>
       </c>
       <c r="H193" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" s="17" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B194" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C194" s="2">
         <v>0</v>
@@ -7566,18 +7578,18 @@
         <v>1</v>
       </c>
       <c r="G194" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H194" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B195" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C195" s="2">
         <v>0</v>
@@ -7595,15 +7607,15 @@
         <v>1</v>
       </c>
       <c r="H195" s="17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B196" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C196" s="2">
         <v>0</v>
@@ -7618,18 +7630,18 @@
         <v>1</v>
       </c>
       <c r="G196" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H196" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197" s="17" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B197" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C197" s="2">
         <v>0</v>
@@ -7647,15 +7659,15 @@
         <v>0</v>
       </c>
       <c r="H197" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B198" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C198" s="2">
         <v>0</v>
@@ -7673,15 +7685,15 @@
         <v>0</v>
       </c>
       <c r="H198" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199" s="17" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B199" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C199" s="2">
         <v>0</v>
@@ -7699,15 +7711,15 @@
         <v>0</v>
       </c>
       <c r="H199" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B200" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C200" s="2">
         <v>0</v>
@@ -7725,15 +7737,15 @@
         <v>0</v>
       </c>
       <c r="H200" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" s="17" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B201" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C201" s="2">
         <v>0</v>
@@ -7751,15 +7763,15 @@
         <v>0</v>
       </c>
       <c r="H201" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" s="17" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B202" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C202" s="2">
         <v>0</v>
@@ -7777,15 +7789,15 @@
         <v>0</v>
       </c>
       <c r="H202" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203" s="17" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B203" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C203" s="2">
         <v>0</v>
@@ -7803,15 +7815,15 @@
         <v>0</v>
       </c>
       <c r="H203" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" s="17" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B204" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C204" s="2">
         <v>0</v>
@@ -7829,15 +7841,15 @@
         <v>0</v>
       </c>
       <c r="H204" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205" s="17" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B205" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C205" s="2">
         <v>0</v>
@@ -7855,15 +7867,15 @@
         <v>0</v>
       </c>
       <c r="H205" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B206" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C206" s="2">
         <v>0</v>
@@ -7881,15 +7893,15 @@
         <v>0</v>
       </c>
       <c r="H206" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B207" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C207" s="2">
         <v>0</v>
@@ -7907,15 +7919,15 @@
         <v>0</v>
       </c>
       <c r="H207" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" s="17" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B208" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C208" s="2">
         <v>0</v>
@@ -7933,15 +7945,15 @@
         <v>0</v>
       </c>
       <c r="H208" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" s="17" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B209" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C209" s="2">
         <v>0</v>
@@ -7959,15 +7971,15 @@
         <v>0</v>
       </c>
       <c r="H209" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" s="17" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B210" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C210" s="2">
         <v>0</v>
@@ -7985,15 +7997,15 @@
         <v>0</v>
       </c>
       <c r="H210" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B211" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C211" s="2">
         <v>0</v>
@@ -8011,15 +8023,15 @@
         <v>0</v>
       </c>
       <c r="H211" s="17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212" s="17" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B212" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C212" s="2">
         <v>0</v>
@@ -8037,15 +8049,15 @@
         <v>0</v>
       </c>
       <c r="H212" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213" s="17" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B213" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C213" s="2">
         <v>0</v>
@@ -8056,22 +8068,22 @@
       <c r="E213" s="20">
         <v>1</v>
       </c>
-      <c r="F213" s="20">
+      <c r="F213" s="22">
         <v>1</v>
       </c>
       <c r="G213" s="3">
         <v>0</v>
       </c>
       <c r="H213" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214" s="17" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B214" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C214" s="2">
         <v>0</v>
@@ -8082,22 +8094,22 @@
       <c r="E214" s="20">
         <v>1</v>
       </c>
-      <c r="F214" s="22">
+      <c r="F214" s="20">
         <v>1</v>
       </c>
       <c r="G214" s="3">
         <v>0</v>
       </c>
       <c r="H214" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215" s="17" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B215" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C215" s="2">
         <v>0</v>
@@ -8115,15 +8127,15 @@
         <v>0</v>
       </c>
       <c r="H215" s="17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A216" s="17" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B216" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C216" s="2">
         <v>0</v>
@@ -8141,15 +8153,15 @@
         <v>0</v>
       </c>
       <c r="H216" s="17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217" s="17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B217" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C217" s="2">
         <v>0</v>
@@ -8167,15 +8179,15 @@
         <v>0</v>
       </c>
       <c r="H217" s="17" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A218" s="17" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B218" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C218" s="2">
         <v>0</v>
@@ -8193,15 +8205,15 @@
         <v>0</v>
       </c>
       <c r="H218" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" s="17" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B219" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C219" s="2">
         <v>0</v>
@@ -8219,15 +8231,15 @@
         <v>0</v>
       </c>
       <c r="H219" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A220" s="17" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B220" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C220" s="2">
         <v>0</v>
@@ -8245,15 +8257,15 @@
         <v>0</v>
       </c>
       <c r="H220" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A221" s="17" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B221" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C221" s="2">
         <v>0</v>
@@ -8271,67 +8283,67 @@
         <v>0</v>
       </c>
       <c r="H221" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A222" s="17" t="s">
+        <v>483</v>
+      </c>
+      <c r="B222" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C222" s="2">
+        <v>0</v>
+      </c>
+      <c r="D222" s="2">
+        <v>0</v>
+      </c>
+      <c r="E222" s="20">
+        <v>1</v>
+      </c>
+      <c r="F222" s="22">
+        <v>1</v>
+      </c>
+      <c r="G222" s="3">
+        <v>0</v>
+      </c>
+      <c r="H222" s="17" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A223" s="17" t="s">
         <v>484</v>
       </c>
-      <c r="B222" s="14" t="s">
+      <c r="B223" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="C222" s="2">
-        <v>0</v>
-      </c>
-      <c r="D222" s="2">
-        <v>0</v>
-      </c>
-      <c r="E222" s="20">
-        <v>1</v>
-      </c>
-      <c r="F222" s="22">
-        <v>1</v>
-      </c>
-      <c r="G222" s="3">
-        <v>0</v>
-      </c>
-      <c r="H222" s="17" t="s">
+      <c r="C223" s="2">
+        <v>0</v>
+      </c>
+      <c r="D223" s="2">
+        <v>0</v>
+      </c>
+      <c r="E223" s="20">
+        <v>1</v>
+      </c>
+      <c r="F223" s="22">
+        <v>1</v>
+      </c>
+      <c r="G223" s="3">
+        <v>0</v>
+      </c>
+      <c r="H223" s="17" t="s">
         <v>325</v>
-      </c>
-    </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A223" s="18" t="s">
-        <v>485</v>
-      </c>
-      <c r="B223" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="C223" s="2">
-        <v>0</v>
-      </c>
-      <c r="D223" s="2">
-        <v>0</v>
-      </c>
-      <c r="E223" s="20">
-        <v>1</v>
-      </c>
-      <c r="F223" s="22">
-        <v>1</v>
-      </c>
-      <c r="G223" s="3">
-        <v>0</v>
-      </c>
-      <c r="H223" s="18" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A224" s="18" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B224" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C224" s="2">
         <v>0</v>
@@ -8349,15 +8361,15 @@
         <v>0</v>
       </c>
       <c r="H224" s="18" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A225" s="18" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B225" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C225" s="2">
         <v>0</v>
@@ -8375,15 +8387,15 @@
         <v>0</v>
       </c>
       <c r="H225" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A226" s="18" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B226" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C226" s="2">
         <v>0</v>
@@ -8401,15 +8413,15 @@
         <v>0</v>
       </c>
       <c r="H226" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A227" s="18" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B227" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C227" s="2">
         <v>0</v>
@@ -8427,15 +8439,15 @@
         <v>0</v>
       </c>
       <c r="H227" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A228" s="18" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B228" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C228" s="2">
         <v>0</v>
@@ -8453,15 +8465,15 @@
         <v>0</v>
       </c>
       <c r="H228" s="18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A229" s="18" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B229" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C229" s="2">
         <v>0</v>
@@ -8479,84 +8491,110 @@
         <v>0</v>
       </c>
       <c r="H229" s="18" t="s">
-        <v>213</v>
+        <v>331</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A230" s="18" t="s">
+        <v>491</v>
+      </c>
+      <c r="B230" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C230" s="2">
+        <v>0</v>
+      </c>
+      <c r="D230" s="2">
+        <v>0</v>
+      </c>
+      <c r="E230" s="20">
+        <v>1</v>
+      </c>
+      <c r="F230" s="22">
+        <v>1</v>
+      </c>
+      <c r="G230" s="3">
+        <v>0</v>
+      </c>
+      <c r="H230" s="18" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A231" s="18" t="s">
         <v>492</v>
       </c>
-      <c r="B230" s="16" t="s">
+      <c r="B231" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="C230" s="2">
-        <v>0</v>
-      </c>
-      <c r="D230" s="2">
-        <v>0</v>
-      </c>
-      <c r="E230" s="20">
-        <v>1</v>
-      </c>
-      <c r="F230" s="20">
-        <v>1</v>
-      </c>
-      <c r="G230" s="3">
-        <v>0</v>
-      </c>
-      <c r="H230" s="18" t="s">
+      <c r="C231" s="2">
+        <v>0</v>
+      </c>
+      <c r="D231" s="2">
+        <v>0</v>
+      </c>
+      <c r="E231" s="20">
+        <v>1</v>
+      </c>
+      <c r="F231" s="20">
+        <v>1</v>
+      </c>
+      <c r="G231" s="3">
+        <v>0</v>
+      </c>
+      <c r="H231" s="18" t="s">
         <v>212</v>
-      </c>
-    </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A231" s="5" t="s">
-        <v>637</v>
-      </c>
-      <c r="B231" s="5" t="s">
-        <v>638</v>
-      </c>
-      <c r="C231" s="2">
-        <v>1</v>
-      </c>
-      <c r="D231" s="2">
-        <v>1</v>
-      </c>
-      <c r="E231" s="4">
-        <v>1</v>
-      </c>
-      <c r="F231" s="3">
-        <v>1</v>
-      </c>
-      <c r="G231" s="3">
-        <v>0</v>
-      </c>
-      <c r="H231" s="5" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A232" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="B232" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="C232" s="2">
+        <v>1</v>
+      </c>
+      <c r="D232" s="2">
+        <v>1</v>
+      </c>
+      <c r="E232" s="4">
+        <v>1</v>
+      </c>
+      <c r="F232" s="3">
+        <v>1</v>
+      </c>
+      <c r="G232" s="3">
+        <v>0</v>
+      </c>
+      <c r="H232" s="5" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A233" s="5" t="s">
         <v>640</v>
       </c>
-      <c r="B232" s="5" t="s">
+      <c r="B233" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="C232" s="2">
-        <v>1</v>
-      </c>
-      <c r="D232" s="2">
-        <v>1</v>
-      </c>
-      <c r="E232" s="2">
-        <v>1</v>
-      </c>
-      <c r="F232" s="2">
-        <v>1</v>
-      </c>
-      <c r="G232" s="2">
-        <v>1</v>
-      </c>
-      <c r="H232" s="5" t="s">
+      <c r="C233" s="2">
+        <v>1</v>
+      </c>
+      <c r="D233" s="2">
+        <v>1</v>
+      </c>
+      <c r="E233" s="2">
+        <v>1</v>
+      </c>
+      <c r="F233" s="2">
+        <v>1</v>
+      </c>
+      <c r="G233" s="2">
+        <v>1</v>
+      </c>
+      <c r="H233" s="5" t="s">
         <v>640</v>
       </c>
     </row>

</xml_diff>